<commit_message>
Separação dos problemas por categorias,modelo II com leitura de arquivo de periodos e fazendo a redução de 10%
</commit_message>
<xml_diff>
--- a/Codes/ModeloAlocacao/dados_experimentos.xlsx
+++ b/Codes/ModeloAlocacao/dados_experimentos.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="macmini_leves" sheetId="2" r:id="rId1"/>
     <sheet name="macbook(ignorar)" sheetId="1" r:id="rId2"/>
+    <sheet name="categorias" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="resultados_1" localSheetId="2">categorias!$A$3:$F$102</definedName>
     <definedName name="resultados_1" localSheetId="1">'macbook(ignorar)'!$H$1:$M$98</definedName>
     <definedName name="resultados_1" localSheetId="0">macmini_leves!$A$1:$F$100</definedName>
     <definedName name="resultados_buffers_leves" localSheetId="1">'macbook(ignorar)'!$A$1:$F$98</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +29,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="resultados_1.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:victormedeiros:Dropbox:trabalho:ufrpe:orientacoes:tcc:workspace:ModeloAlocacao:resultados_1.txt" decimal="," thousands="." delimiter=":">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:victormedeiros:Dropbox:trabalho:ufrpe:orientacoes:tcc:workspace:ModeloAlocacao:resultados_1.txt" decimal="," thousands="." delimiter=":">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -37,8 +39,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="resultados_buffers_leves.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:victormedeiros:Dropbox:trabalho:ufrpe:orientacoes:tcc:workspace:ModeloAlocacao:resultados_buffers_leves.txt" decimal="," thousands="." delimiter=":">
+  <connection id="2" name="resultados_1.txt2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:victormedeiros:Dropbox:trabalho:ufrpe:orientacoes:tcc:workspace:ModeloAlocacao:resultados_1.txt" decimal="," thousands="." delimiter=":">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="resultados_buffers_leves.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:victormedeiros:Dropbox:trabalho:ufrpe:orientacoes:tcc:workspace:ModeloAlocacao:resultados_buffers_leves.txt" decimal="," thousands="." delimiter=":">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -53,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="6">
   <si>
     <t>f</t>
   </si>
@@ -63,12 +76,21 @@
   <si>
     <t>d</t>
   </si>
+  <si>
+    <t>Facil</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>Difícil</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,12 +151,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink seguido" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -151,7 +173,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="resultados_buffers_leves" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="resultados_buffers_leves" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="resultados_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,20 +501,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2504,26 +2530,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -6258,4 +6284,1933 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="12" max="12" width="15.625" customWidth="1"/>
+    <col min="19" max="19" width="16.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>68.17</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>34.69</v>
+      </c>
+      <c r="K2">
+        <v>400</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1E-3</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>18.87</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>70.52</v>
+      </c>
+      <c r="D3">
+        <v>400</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>47.63</v>
+      </c>
+      <c r="K3">
+        <v>225.99</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>15.56</v>
+      </c>
+      <c r="R3">
+        <v>400</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>87.88</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>34.53</v>
+      </c>
+      <c r="K4">
+        <v>273.07</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
+      <c r="P4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>28.95</v>
+      </c>
+      <c r="R4">
+        <v>225.02</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>97.08</v>
+      </c>
+      <c r="D5">
+        <v>400</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>20.7</v>
+      </c>
+      <c r="K5">
+        <v>354.25</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="O5">
+        <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>28.87</v>
+      </c>
+      <c r="R5">
+        <v>179.55</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>337.43200000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>66.56</v>
+      </c>
+      <c r="D6">
+        <v>400</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>80.959999999999994</v>
+      </c>
+      <c r="K6">
+        <v>364.09</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>3.4820000000000002</v>
+      </c>
+      <c r="O6">
+        <v>14</v>
+      </c>
+      <c r="P6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>13.72</v>
+      </c>
+      <c r="R6">
+        <v>400</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>92.82</v>
+      </c>
+      <c r="D7">
+        <v>400</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>60.78</v>
+      </c>
+      <c r="K7">
+        <v>400</v>
+      </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0.03</v>
+      </c>
+      <c r="O7">
+        <v>15</v>
+      </c>
+      <c r="P7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>44.78</v>
+      </c>
+      <c r="R7">
+        <v>273.07</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>72564.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>66.16</v>
+      </c>
+      <c r="D8">
+        <v>400</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2E-3</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>29.1</v>
+      </c>
+      <c r="K8">
+        <v>400</v>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O8">
+        <v>18</v>
+      </c>
+      <c r="P8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>13.1</v>
+      </c>
+      <c r="R8">
+        <v>159.84</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0.63700000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>67.03</v>
+      </c>
+      <c r="D9">
+        <v>400</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>51.74</v>
+      </c>
+      <c r="K9">
+        <v>400</v>
+      </c>
+      <c r="L9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>2E-3</v>
+      </c>
+      <c r="O9">
+        <v>24</v>
+      </c>
+      <c r="P9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>13.05</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>86.43</v>
+      </c>
+      <c r="D10">
+        <v>400</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1E-3</v>
+      </c>
+      <c r="H10">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>44.11</v>
+      </c>
+      <c r="K10">
+        <v>400</v>
+      </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>2E-3</v>
+      </c>
+      <c r="O10">
+        <v>32</v>
+      </c>
+      <c r="P10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>11.43</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>60.51</v>
+      </c>
+      <c r="D11">
+        <v>400</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>46.91</v>
+      </c>
+      <c r="K11">
+        <v>400</v>
+      </c>
+      <c r="L11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="O11">
+        <v>41</v>
+      </c>
+      <c r="P11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>48.61</v>
+      </c>
+      <c r="R11">
+        <v>272.36</v>
+      </c>
+      <c r="S11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>338.43700000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>82.37</v>
+      </c>
+      <c r="D12">
+        <v>400</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2E-3</v>
+      </c>
+      <c r="H12">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>48.56</v>
+      </c>
+      <c r="K12">
+        <v>400</v>
+      </c>
+      <c r="L12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O12">
+        <v>46</v>
+      </c>
+      <c r="P12" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>19.53</v>
+      </c>
+      <c r="R12">
+        <v>400</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>70.06</v>
+      </c>
+      <c r="D13">
+        <v>400</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>2E-3</v>
+      </c>
+      <c r="H13">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>60.01</v>
+      </c>
+      <c r="K13">
+        <v>297.89</v>
+      </c>
+      <c r="L13" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="O13">
+        <v>48</v>
+      </c>
+      <c r="P13" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>18.61</v>
+      </c>
+      <c r="R13">
+        <v>204.8</v>
+      </c>
+      <c r="S13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>0.56799999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>62.42</v>
+      </c>
+      <c r="D14">
+        <v>400</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H14">
+        <v>25</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>40.229999999999997</v>
+      </c>
+      <c r="K14">
+        <v>327.68</v>
+      </c>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="O14">
+        <v>52</v>
+      </c>
+      <c r="P14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>63.95</v>
+      </c>
+      <c r="R14">
+        <v>364.09</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1995.2739999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>79.3</v>
+      </c>
+      <c r="D15">
+        <v>400</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H15">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>21.18</v>
+      </c>
+      <c r="K15">
+        <v>400</v>
+      </c>
+      <c r="L15" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O15">
+        <v>53</v>
+      </c>
+      <c r="P15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>11.68</v>
+      </c>
+      <c r="R15">
+        <v>242.73</v>
+      </c>
+      <c r="S15" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>12.29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>83.44</v>
+      </c>
+      <c r="D16">
+        <v>400</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H16">
+        <v>27</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>54.28</v>
+      </c>
+      <c r="K16">
+        <v>204.8</v>
+      </c>
+      <c r="L16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>16054.233</v>
+      </c>
+      <c r="O16">
+        <v>57</v>
+      </c>
+      <c r="P16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>19.75</v>
+      </c>
+      <c r="R16">
+        <v>273.07</v>
+      </c>
+      <c r="S16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>95.48</v>
+      </c>
+      <c r="D17">
+        <v>400</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H17">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>62.15</v>
+      </c>
+      <c r="K17">
+        <v>354.25</v>
+      </c>
+      <c r="L17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>13.885999999999999</v>
+      </c>
+      <c r="O17">
+        <v>58</v>
+      </c>
+      <c r="P17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17">
+        <v>18.82</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="b">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>74.41</v>
+      </c>
+      <c r="D18">
+        <v>364.09</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>3.9E-2</v>
+      </c>
+      <c r="H18">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="K18">
+        <v>297.89</v>
+      </c>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="O18">
+        <v>60</v>
+      </c>
+      <c r="P18" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>19.34</v>
+      </c>
+      <c r="R18">
+        <v>400</v>
+      </c>
+      <c r="S18" t="b">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>91.99</v>
+      </c>
+      <c r="D19">
+        <v>400</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>2E-3</v>
+      </c>
+      <c r="H19">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>67.239999999999995</v>
+      </c>
+      <c r="K19">
+        <v>204.8</v>
+      </c>
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="O19">
+        <v>62</v>
+      </c>
+      <c r="P19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q19">
+        <v>48.14</v>
+      </c>
+      <c r="R19">
+        <v>204.8</v>
+      </c>
+      <c r="S19" t="b">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>3.2639999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="D20">
+        <v>400</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2E-3</v>
+      </c>
+      <c r="H20">
+        <v>34</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>37.85</v>
+      </c>
+      <c r="K20">
+        <v>400</v>
+      </c>
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O20">
+        <v>79</v>
+      </c>
+      <c r="P20" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>16.5</v>
+      </c>
+      <c r="R20">
+        <v>291.27</v>
+      </c>
+      <c r="S20" t="b">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>160.703</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>77.55</v>
+      </c>
+      <c r="D21">
+        <v>400</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H21">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>33.89</v>
+      </c>
+      <c r="K21">
+        <v>311.16000000000003</v>
+      </c>
+      <c r="L21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="O21">
+        <v>80</v>
+      </c>
+      <c r="P21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <v>11.71</v>
+      </c>
+      <c r="R21">
+        <v>229.95</v>
+      </c>
+      <c r="S21" t="b">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>0.17299999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>85.08</v>
+      </c>
+      <c r="D22">
+        <v>400</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>36</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>52.39</v>
+      </c>
+      <c r="K22">
+        <v>312.08</v>
+      </c>
+      <c r="L22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="O22">
+        <v>85</v>
+      </c>
+      <c r="P22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>18.78</v>
+      </c>
+      <c r="R22">
+        <v>400</v>
+      </c>
+      <c r="S22" t="b">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>75.95</v>
+      </c>
+      <c r="D23">
+        <v>400</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H23">
+        <v>37</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>46.23</v>
+      </c>
+      <c r="K23">
+        <v>400</v>
+      </c>
+      <c r="L23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>2E-3</v>
+      </c>
+      <c r="O23">
+        <v>86</v>
+      </c>
+      <c r="P23" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>38.56</v>
+      </c>
+      <c r="R23">
+        <v>182.04</v>
+      </c>
+      <c r="S23" t="b">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>80.040000000000006</v>
+      </c>
+      <c r="D24">
+        <v>400</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H24">
+        <v>38</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>24.79</v>
+      </c>
+      <c r="K24">
+        <v>311.16000000000003</v>
+      </c>
+      <c r="L24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O24">
+        <v>96</v>
+      </c>
+      <c r="P24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24">
+        <v>4.5</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>2.0680000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>82.65</v>
+      </c>
+      <c r="D25">
+        <v>400</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>42</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>27.93</v>
+      </c>
+      <c r="K25">
+        <v>400</v>
+      </c>
+      <c r="L25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O25">
+        <v>99</v>
+      </c>
+      <c r="P25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q25">
+        <v>48.12</v>
+      </c>
+      <c r="R25">
+        <v>273.07</v>
+      </c>
+      <c r="S25" t="b">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>2.9249999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>94.12</v>
+      </c>
+      <c r="D26">
+        <v>400</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>43</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>56.92</v>
+      </c>
+      <c r="K26">
+        <v>400</v>
+      </c>
+      <c r="L26" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>66.05</v>
+      </c>
+      <c r="D27">
+        <v>400</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H27">
+        <v>44</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>61.25</v>
+      </c>
+      <c r="K27">
+        <v>291.27</v>
+      </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1131.835</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>71.680000000000007</v>
+      </c>
+      <c r="D28">
+        <v>400</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H28">
+        <v>45</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>48.47</v>
+      </c>
+      <c r="K28">
+        <v>400</v>
+      </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="H29">
+        <v>47</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>41.02</v>
+      </c>
+      <c r="K29">
+        <v>400</v>
+      </c>
+      <c r="L29" t="b">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="H30">
+        <v>50</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>69.05</v>
+      </c>
+      <c r="K30">
+        <v>267.49</v>
+      </c>
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="H31">
+        <v>51</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>43.92</v>
+      </c>
+      <c r="K31">
+        <v>400</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="H32">
+        <v>54</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>37.74</v>
+      </c>
+      <c r="K32">
+        <v>91.02</v>
+      </c>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="8:13">
+      <c r="H33">
+        <v>55</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>66.23</v>
+      </c>
+      <c r="K33">
+        <v>267.49</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>2065.549</v>
+      </c>
+    </row>
+    <row r="34" spans="8:13">
+      <c r="H34">
+        <v>65</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>31.25</v>
+      </c>
+      <c r="K34">
+        <v>400</v>
+      </c>
+      <c r="L34" t="b">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="8:13">
+      <c r="H35">
+        <v>66</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>42.68</v>
+      </c>
+      <c r="K35">
+        <v>400</v>
+      </c>
+      <c r="L35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="8:13">
+      <c r="H36">
+        <v>67</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>47.82</v>
+      </c>
+      <c r="K36">
+        <v>400</v>
+      </c>
+      <c r="L36" t="b">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="8:13">
+      <c r="H37">
+        <v>68</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>68.540000000000006</v>
+      </c>
+      <c r="K37">
+        <v>400</v>
+      </c>
+      <c r="L37" t="b">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="8:13">
+      <c r="H38">
+        <v>69</v>
+      </c>
+      <c r="I38" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>32.07</v>
+      </c>
+      <c r="K38">
+        <v>400</v>
+      </c>
+      <c r="L38" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="8:13">
+      <c r="H39">
+        <v>72</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>54.55</v>
+      </c>
+      <c r="K39">
+        <v>148.94999999999999</v>
+      </c>
+      <c r="L39" t="b">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="8:13">
+      <c r="H40">
+        <v>73</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>29.28</v>
+      </c>
+      <c r="K40">
+        <v>400</v>
+      </c>
+      <c r="L40" t="b">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="8:13">
+      <c r="H41">
+        <v>74</v>
+      </c>
+      <c r="I41" t="s">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>37.82</v>
+      </c>
+      <c r="K41">
+        <v>310.24</v>
+      </c>
+      <c r="L41" t="b">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="8:13">
+      <c r="H42">
+        <v>75</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>24.94</v>
+      </c>
+      <c r="K42">
+        <v>400</v>
+      </c>
+      <c r="L42" t="b">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="8:13">
+      <c r="H43">
+        <v>77</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>35.14</v>
+      </c>
+      <c r="K43">
+        <v>400</v>
+      </c>
+      <c r="L43" t="b">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="8:13">
+      <c r="H44">
+        <v>82</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>55.38</v>
+      </c>
+      <c r="K44">
+        <v>400</v>
+      </c>
+      <c r="L44" t="b">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="8:13">
+      <c r="H45">
+        <v>83</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>60.61</v>
+      </c>
+      <c r="K45">
+        <v>272.70999999999998</v>
+      </c>
+      <c r="L45" t="b">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="8:13">
+      <c r="H46">
+        <v>87</v>
+      </c>
+      <c r="I46" t="s">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>52.1</v>
+      </c>
+      <c r="K46">
+        <v>364.09</v>
+      </c>
+      <c r="L46" t="b">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="47" spans="8:13">
+      <c r="H47">
+        <v>90</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>57.32</v>
+      </c>
+      <c r="K47">
+        <v>400</v>
+      </c>
+      <c r="L47" t="b">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="8:13">
+      <c r="H48">
+        <v>91</v>
+      </c>
+      <c r="I48" t="s">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>42.15</v>
+      </c>
+      <c r="K48">
+        <v>354.25</v>
+      </c>
+      <c r="L48" t="b">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>12.581</v>
+      </c>
+    </row>
+    <row r="49" spans="8:13">
+      <c r="H49">
+        <v>94</v>
+      </c>
+      <c r="I49" t="s">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>39.99</v>
+      </c>
+      <c r="K49">
+        <v>327.68</v>
+      </c>
+      <c r="L49" t="b">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1.4219999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="8:13">
+      <c r="H50">
+        <v>98</v>
+      </c>
+      <c r="I50" t="s">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>66.86</v>
+      </c>
+      <c r="K50">
+        <v>252.06</v>
+      </c>
+      <c r="L50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>